<commit_message>
Cren regio -> G5, update a few G4 samples
</commit_message>
<xml_diff>
--- a/data/processed/CascadiaMargin_carbon_abundance.xlsx
+++ b/data/processed/CascadiaMargin_carbon_abundance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinekeller/Desktop/cascadia-margin-lipids/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF1CADF-D0D0-BC49-858E-F7D47916246C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684CEDF1-64DC-724E-98A0-E40A6206889F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="32200" windowHeight="22080" xr2:uid="{5EB331C3-10DF-C24A-ADC1-4DCB6056C63D}"/>
+    <workbookView xWindow="16560" yWindow="500" windowWidth="21840" windowHeight="22000" xr2:uid="{5EB331C3-10DF-C24A-ADC1-4DCB6056C63D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,13 +216,13 @@
     <t>d13c_avg</t>
   </si>
   <si>
-    <t>Cren regio</t>
-  </si>
-  <si>
     <t>S3</t>
   </si>
   <si>
     <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
   </si>
 </sst>
 </file>
@@ -641,7 +641,7 @@
   <dimension ref="A1:XEP260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -854,7 +854,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="7"/>
@@ -874,7 +874,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D8" s="8">
         <v>20</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="9" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16370">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>4</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="10" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16370">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>4</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="11" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16370">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>4</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="12" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16370">
       <c r="A12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>4</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="13" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16370">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>4</v>
@@ -1012,13 +1012,13 @@
     </row>
     <row r="14" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16370">
       <c r="A14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="7"/>
@@ -1032,13 +1032,13 @@
     </row>
     <row r="15" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16370" s="10" customFormat="1">
       <c r="A15" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D15" s="8">
         <v>20</v>
@@ -3258,7 +3258,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="7"/>
@@ -3278,7 +3278,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D22" s="8">
         <v>20</v>
@@ -3476,7 +3476,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7"/>
@@ -3498,7 +3498,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D29" s="8">
         <v>20</v>
@@ -3678,7 +3678,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="7"/>
@@ -3699,7 +3699,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D36" s="8">
         <v>0</v>
@@ -3889,7 +3889,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="7"/>
@@ -3910,7 +3910,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D43" s="8">
         <v>0</v>
@@ -4100,7 +4100,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="7"/>
@@ -4121,7 +4121,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D50" s="8">
         <v>0</v>
@@ -4321,7 +4321,7 @@
         <v>4</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="7"/>
@@ -4341,7 +4341,7 @@
         <v>4</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D57" s="8">
         <v>0</v>
@@ -4529,7 +4529,7 @@
         <v>21</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="7"/>
@@ -4549,7 +4549,7 @@
         <v>21</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D64" s="8">
         <v>0</v>
@@ -4737,7 +4737,7 @@
         <v>21</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="7"/>
@@ -4757,7 +4757,7 @@
         <v>21</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D71" s="8">
         <v>0</v>
@@ -4945,7 +4945,7 @@
         <v>21</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D77" s="8"/>
       <c r="E77" s="7"/>
@@ -4965,7 +4965,7 @@
         <v>21</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D78" s="8">
         <v>0</v>
@@ -5153,7 +5153,7 @@
         <v>21</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="7"/>
@@ -5173,7 +5173,7 @@
         <v>21</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D85" s="8">
         <v>0</v>
@@ -5361,7 +5361,7 @@
         <v>21</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="7"/>
@@ -5381,7 +5381,7 @@
         <v>21</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D92" s="8">
         <v>10</v>
@@ -5569,7 +5569,7 @@
         <v>21</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="7"/>
@@ -5589,7 +5589,7 @@
         <v>21</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D99" s="8">
         <v>10</v>
@@ -5777,7 +5777,7 @@
         <v>21</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="7"/>
@@ -5797,7 +5797,7 @@
         <v>21</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D106" s="8">
         <v>10</v>
@@ -5985,7 +5985,7 @@
         <v>21</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="7"/>
@@ -6005,7 +6005,7 @@
         <v>21</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D113" s="8">
         <v>10</v>
@@ -6193,7 +6193,7 @@
         <v>21</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="7"/>
@@ -6213,7 +6213,7 @@
         <v>21</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D120" s="8">
         <v>60</v>
@@ -6401,7 +6401,7 @@
         <v>21</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="7"/>
@@ -6421,7 +6421,7 @@
         <v>21</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D127" s="8">
         <v>60</v>
@@ -6609,7 +6609,7 @@
         <v>21</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D133" s="8"/>
       <c r="E133" s="7"/>
@@ -6629,7 +6629,7 @@
         <v>21</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D134" s="8">
         <v>60</v>
@@ -6817,7 +6817,7 @@
         <v>21</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="7"/>
@@ -6837,7 +6837,7 @@
         <v>21</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D141" s="8">
         <v>60</v>
@@ -7025,7 +7025,7 @@
         <v>21</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D147" s="8"/>
       <c r="E147" s="7"/>
@@ -7045,7 +7045,7 @@
         <v>21</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D148" s="8">
         <v>30</v>
@@ -7233,7 +7233,7 @@
         <v>21</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D154" s="8"/>
       <c r="E154" s="7"/>
@@ -7253,7 +7253,7 @@
         <v>21</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D155" s="8">
         <v>30</v>
@@ -7441,7 +7441,7 @@
         <v>21</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D161" s="8"/>
       <c r="E161" s="7"/>
@@ -7461,7 +7461,7 @@
         <v>21</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D162" s="8">
         <v>30</v>
@@ -7649,7 +7649,7 @@
         <v>21</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D168" s="8"/>
       <c r="E168" s="7"/>
@@ -7669,7 +7669,7 @@
         <v>21</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D169" s="8">
         <v>30</v>
@@ -7835,7 +7835,7 @@
         <v>38</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D175" s="8"/>
       <c r="E175" s="7"/>
@@ -7855,7 +7855,7 @@
         <v>38</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D176" s="8">
         <v>15</v>
@@ -8021,7 +8021,7 @@
         <v>38</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D182" s="8"/>
       <c r="E182" s="7"/>
@@ -8041,7 +8041,7 @@
         <v>38</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D183" s="8">
         <v>30</v>
@@ -8207,7 +8207,7 @@
         <v>38</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D189" s="8"/>
       <c r="E189" s="7"/>
@@ -8227,7 +8227,7 @@
         <v>38</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D190" s="8">
         <v>30</v>
@@ -8393,7 +8393,7 @@
         <v>38</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D196" s="8"/>
       <c r="E196" s="7"/>
@@ -8413,7 +8413,7 @@
         <v>38</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D197" s="8">
         <v>30</v>
@@ -8601,7 +8601,7 @@
         <v>38</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D203" s="8"/>
       <c r="E203" s="7"/>
@@ -8621,7 +8621,7 @@
         <v>38</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D204" s="8">
         <v>30</v>
@@ -8787,7 +8787,7 @@
         <v>38</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D210" s="8"/>
       <c r="E210" s="7"/>
@@ -8807,7 +8807,7 @@
         <v>38</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D211" s="8">
         <v>60</v>
@@ -8983,7 +8983,7 @@
         <v>38</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D217" s="8"/>
       <c r="E217" s="7"/>
@@ -9005,7 +9005,7 @@
         <v>38</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D218" s="8">
         <v>60</v>
@@ -9173,7 +9173,7 @@
         <v>38</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="7"/>
@@ -9193,7 +9193,7 @@
         <v>38</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D225" s="8">
         <v>60</v>
@@ -9381,7 +9381,7 @@
         <v>38</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D231" s="8"/>
       <c r="E231" s="7"/>
@@ -9401,7 +9401,7 @@
         <v>38</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D232" s="8">
         <v>60</v>
@@ -9567,7 +9567,7 @@
         <v>38</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="7"/>
@@ -9587,7 +9587,7 @@
         <v>38</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D239" s="8">
         <v>0</v>
@@ -9753,7 +9753,7 @@
         <v>38</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D245" s="8"/>
       <c r="E245" s="7"/>
@@ -9773,7 +9773,7 @@
         <v>38</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D246" s="8">
         <v>0</v>
@@ -9939,7 +9939,7 @@
         <v>38</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D252" s="8"/>
       <c r="E252" s="7"/>
@@ -9959,7 +9959,7 @@
         <v>38</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D253" s="8">
         <v>0</v>
@@ -10143,7 +10143,7 @@
         <v>38</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D259" s="8"/>
       <c r="E259" s="7"/>
@@ -10159,7 +10159,7 @@
         <v>38</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D260" s="8">
         <v>0</v>

</xml_diff>